<commit_message>
Updated for older Matlab
</commit_message>
<xml_diff>
--- a/databank/toXLSUnitTest.xlsx
+++ b/databank/toXLSUnitTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5357" uniqueCount="5357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6176" uniqueCount="6176">
   <si>
     <t>2022-Feb-05</t>
   </si>
@@ -16075,6 +16075,2463 @@
   </si>
   <si>
     <t>2022-Sep-15</t>
+  </si>
+  <si>
+    <t>daily1</t>
+  </si>
+  <si>
+    <t>daily2</t>
+  </si>
+  <si>
+    <t>daily3</t>
+  </si>
+  <si>
+    <t>daily4</t>
+  </si>
+  <si>
+    <t>daily5</t>
+  </si>
+  <si>
+    <t>2023Y</t>
+  </si>
+  <si>
+    <t>2024Y</t>
+  </si>
+  <si>
+    <t>2025Y</t>
+  </si>
+  <si>
+    <t>2026Y</t>
+  </si>
+  <si>
+    <t>2027Y</t>
+  </si>
+  <si>
+    <t>2028Y</t>
+  </si>
+  <si>
+    <t>2029Y</t>
+  </si>
+  <si>
+    <t>2030Y</t>
+  </si>
+  <si>
+    <t>2031Y</t>
+  </si>
+  <si>
+    <t>2032Y</t>
+  </si>
+  <si>
+    <t>2033Y</t>
+  </si>
+  <si>
+    <t>2034Y</t>
+  </si>
+  <si>
+    <t>2035Y</t>
+  </si>
+  <si>
+    <t>2036Y</t>
+  </si>
+  <si>
+    <t>2037Y</t>
+  </si>
+  <si>
+    <t>2038Y</t>
+  </si>
+  <si>
+    <t>2039Y</t>
+  </si>
+  <si>
+    <t>2040Y</t>
+  </si>
+  <si>
+    <t>2041Y</t>
+  </si>
+  <si>
+    <t>yearly1</t>
+  </si>
+  <si>
+    <t>yearly2</t>
+  </si>
+  <si>
+    <t>yearly3</t>
+  </si>
+  <si>
+    <t>yearly4</t>
+  </si>
+  <si>
+    <t>yearly5</t>
+  </si>
+  <si>
+    <t>2023H1</t>
+  </si>
+  <si>
+    <t>2023H2</t>
+  </si>
+  <si>
+    <t>2024H1</t>
+  </si>
+  <si>
+    <t>2024H2</t>
+  </si>
+  <si>
+    <t>2025H1</t>
+  </si>
+  <si>
+    <t>2025H2</t>
+  </si>
+  <si>
+    <t>2026H1</t>
+  </si>
+  <si>
+    <t>2026H2</t>
+  </si>
+  <si>
+    <t>2027H1</t>
+  </si>
+  <si>
+    <t>2027H2</t>
+  </si>
+  <si>
+    <t>2028H1</t>
+  </si>
+  <si>
+    <t>2028H2</t>
+  </si>
+  <si>
+    <t>2029H1</t>
+  </si>
+  <si>
+    <t>2029H2</t>
+  </si>
+  <si>
+    <t>2030H1</t>
+  </si>
+  <si>
+    <t>halfyearly1</t>
+  </si>
+  <si>
+    <t>halfyearly2</t>
+  </si>
+  <si>
+    <t>halfyearly3</t>
+  </si>
+  <si>
+    <t>halfyearly4</t>
+  </si>
+  <si>
+    <t>halfyearly5</t>
+  </si>
+  <si>
+    <t>2022Q4</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>quarterly1</t>
+  </si>
+  <si>
+    <t>quarterly2</t>
+  </si>
+  <si>
+    <t>quarterly3</t>
+  </si>
+  <si>
+    <t>quarterly4</t>
+  </si>
+  <si>
+    <t>quarterly5</t>
+  </si>
+  <si>
+    <t>2022M10</t>
+  </si>
+  <si>
+    <t>2022M11</t>
+  </si>
+  <si>
+    <t>2022M12</t>
+  </si>
+  <si>
+    <t>2023M01</t>
+  </si>
+  <si>
+    <t>2023M02</t>
+  </si>
+  <si>
+    <t>2023M03</t>
+  </si>
+  <si>
+    <t>2023M04</t>
+  </si>
+  <si>
+    <t>2023M05</t>
+  </si>
+  <si>
+    <t>2023M06</t>
+  </si>
+  <si>
+    <t>2023M07</t>
+  </si>
+  <si>
+    <t>2023M08</t>
+  </si>
+  <si>
+    <t>2023M09</t>
+  </si>
+  <si>
+    <t>monthly1</t>
+  </si>
+  <si>
+    <t>monthly2</t>
+  </si>
+  <si>
+    <t>monthly3</t>
+  </si>
+  <si>
+    <t>monthly4</t>
+  </si>
+  <si>
+    <t>monthly5</t>
+  </si>
+  <si>
+    <t>2022W39</t>
+  </si>
+  <si>
+    <t>2022W40</t>
+  </si>
+  <si>
+    <t>2022W41</t>
+  </si>
+  <si>
+    <t>2022W42</t>
+  </si>
+  <si>
+    <t>2022W43</t>
+  </si>
+  <si>
+    <t>2022W44</t>
+  </si>
+  <si>
+    <t>2022W45</t>
+  </si>
+  <si>
+    <t>2022W46</t>
+  </si>
+  <si>
+    <t>2022W47</t>
+  </si>
+  <si>
+    <t>2022W48</t>
+  </si>
+  <si>
+    <t>2022W49</t>
+  </si>
+  <si>
+    <t>2022W50</t>
+  </si>
+  <si>
+    <t>2022W51</t>
+  </si>
+  <si>
+    <t>2022W52</t>
+  </si>
+  <si>
+    <t>2023W01</t>
+  </si>
+  <si>
+    <t>2023W02</t>
+  </si>
+  <si>
+    <t>weekly1</t>
+  </si>
+  <si>
+    <t>weekly2</t>
+  </si>
+  <si>
+    <t>weekly3</t>
+  </si>
+  <si>
+    <t>weekly4</t>
+  </si>
+  <si>
+    <t>weekly5</t>
+  </si>
+  <si>
+    <t>2022-Sep-16</t>
+  </si>
+  <si>
+    <t>2022-Sep-17</t>
+  </si>
+  <si>
+    <t>2022-Sep-18</t>
+  </si>
+  <si>
+    <t>2022-Sep-19</t>
+  </si>
+  <si>
+    <t>2022-Sep-20</t>
+  </si>
+  <si>
+    <t>2022-Sep-21</t>
+  </si>
+  <si>
+    <t>2022-Sep-22</t>
+  </si>
+  <si>
+    <t>2022-Sep-23</t>
+  </si>
+  <si>
+    <t>2022-Sep-24</t>
+  </si>
+  <si>
+    <t>2022-Sep-25</t>
+  </si>
+  <si>
+    <t>2022-Sep-26</t>
+  </si>
+  <si>
+    <t>2022-Sep-27</t>
+  </si>
+  <si>
+    <t>2022-Sep-28</t>
+  </si>
+  <si>
+    <t>2022-Sep-29</t>
+  </si>
+  <si>
+    <t>2022-Sep-30</t>
+  </si>
+  <si>
+    <t>daily1</t>
+  </si>
+  <si>
+    <t>daily2</t>
+  </si>
+  <si>
+    <t>daily3</t>
+  </si>
+  <si>
+    <t>daily4</t>
+  </si>
+  <si>
+    <t>daily5</t>
+  </si>
+  <si>
+    <t>2023Y</t>
+  </si>
+  <si>
+    <t>2024Y</t>
+  </si>
+  <si>
+    <t>2025Y</t>
+  </si>
+  <si>
+    <t>2026Y</t>
+  </si>
+  <si>
+    <t>2027Y</t>
+  </si>
+  <si>
+    <t>2028Y</t>
+  </si>
+  <si>
+    <t>2029Y</t>
+  </si>
+  <si>
+    <t>2030Y</t>
+  </si>
+  <si>
+    <t>2031Y</t>
+  </si>
+  <si>
+    <t>2032Y</t>
+  </si>
+  <si>
+    <t>2033Y</t>
+  </si>
+  <si>
+    <t>2034Y</t>
+  </si>
+  <si>
+    <t>2035Y</t>
+  </si>
+  <si>
+    <t>2036Y</t>
+  </si>
+  <si>
+    <t>2037Y</t>
+  </si>
+  <si>
+    <t>2038Y</t>
+  </si>
+  <si>
+    <t>2039Y</t>
+  </si>
+  <si>
+    <t>2040Y</t>
+  </si>
+  <si>
+    <t>2041Y</t>
+  </si>
+  <si>
+    <t>yearly1</t>
+  </si>
+  <si>
+    <t>yearly2</t>
+  </si>
+  <si>
+    <t>yearly3</t>
+  </si>
+  <si>
+    <t>yearly4</t>
+  </si>
+  <si>
+    <t>yearly5</t>
+  </si>
+  <si>
+    <t>2023H1</t>
+  </si>
+  <si>
+    <t>2023H2</t>
+  </si>
+  <si>
+    <t>2024H1</t>
+  </si>
+  <si>
+    <t>2024H2</t>
+  </si>
+  <si>
+    <t>2025H1</t>
+  </si>
+  <si>
+    <t>2025H2</t>
+  </si>
+  <si>
+    <t>2026H1</t>
+  </si>
+  <si>
+    <t>2026H2</t>
+  </si>
+  <si>
+    <t>2027H1</t>
+  </si>
+  <si>
+    <t>2027H2</t>
+  </si>
+  <si>
+    <t>2028H1</t>
+  </si>
+  <si>
+    <t>2028H2</t>
+  </si>
+  <si>
+    <t>2029H1</t>
+  </si>
+  <si>
+    <t>2029H2</t>
+  </si>
+  <si>
+    <t>2030H1</t>
+  </si>
+  <si>
+    <t>halfyearly1</t>
+  </si>
+  <si>
+    <t>halfyearly2</t>
+  </si>
+  <si>
+    <t>halfyearly3</t>
+  </si>
+  <si>
+    <t>halfyearly4</t>
+  </si>
+  <si>
+    <t>halfyearly5</t>
+  </si>
+  <si>
+    <t>2022Q4</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>quarterly1</t>
+  </si>
+  <si>
+    <t>quarterly2</t>
+  </si>
+  <si>
+    <t>quarterly3</t>
+  </si>
+  <si>
+    <t>quarterly4</t>
+  </si>
+  <si>
+    <t>quarterly5</t>
+  </si>
+  <si>
+    <t>2022M10</t>
+  </si>
+  <si>
+    <t>2022M11</t>
+  </si>
+  <si>
+    <t>2022M12</t>
+  </si>
+  <si>
+    <t>2023M01</t>
+  </si>
+  <si>
+    <t>2023M02</t>
+  </si>
+  <si>
+    <t>2023M03</t>
+  </si>
+  <si>
+    <t>2023M04</t>
+  </si>
+  <si>
+    <t>2023M05</t>
+  </si>
+  <si>
+    <t>2023M06</t>
+  </si>
+  <si>
+    <t>2023M07</t>
+  </si>
+  <si>
+    <t>2023M08</t>
+  </si>
+  <si>
+    <t>2023M09</t>
+  </si>
+  <si>
+    <t>monthly1</t>
+  </si>
+  <si>
+    <t>monthly2</t>
+  </si>
+  <si>
+    <t>monthly3</t>
+  </si>
+  <si>
+    <t>monthly4</t>
+  </si>
+  <si>
+    <t>monthly5</t>
+  </si>
+  <si>
+    <t>2022W39</t>
+  </si>
+  <si>
+    <t>2022W40</t>
+  </si>
+  <si>
+    <t>2022W41</t>
+  </si>
+  <si>
+    <t>2022W42</t>
+  </si>
+  <si>
+    <t>2022W43</t>
+  </si>
+  <si>
+    <t>2022W44</t>
+  </si>
+  <si>
+    <t>2022W45</t>
+  </si>
+  <si>
+    <t>2022W46</t>
+  </si>
+  <si>
+    <t>2022W47</t>
+  </si>
+  <si>
+    <t>2022W48</t>
+  </si>
+  <si>
+    <t>2022W49</t>
+  </si>
+  <si>
+    <t>2022W50</t>
+  </si>
+  <si>
+    <t>2022W51</t>
+  </si>
+  <si>
+    <t>2022W52</t>
+  </si>
+  <si>
+    <t>2023W01</t>
+  </si>
+  <si>
+    <t>2023W02</t>
+  </si>
+  <si>
+    <t>weekly1</t>
+  </si>
+  <si>
+    <t>weekly2</t>
+  </si>
+  <si>
+    <t>weekly3</t>
+  </si>
+  <si>
+    <t>weekly4</t>
+  </si>
+  <si>
+    <t>weekly5</t>
+  </si>
+  <si>
+    <t>2022-Sep-16</t>
+  </si>
+  <si>
+    <t>2022-Sep-17</t>
+  </si>
+  <si>
+    <t>2022-Sep-18</t>
+  </si>
+  <si>
+    <t>2022-Sep-19</t>
+  </si>
+  <si>
+    <t>2022-Sep-20</t>
+  </si>
+  <si>
+    <t>2022-Sep-21</t>
+  </si>
+  <si>
+    <t>2022-Sep-22</t>
+  </si>
+  <si>
+    <t>2022-Sep-23</t>
+  </si>
+  <si>
+    <t>2022-Sep-24</t>
+  </si>
+  <si>
+    <t>2022-Sep-25</t>
+  </si>
+  <si>
+    <t>2022-Sep-26</t>
+  </si>
+  <si>
+    <t>2022-Sep-27</t>
+  </si>
+  <si>
+    <t>2022-Sep-28</t>
+  </si>
+  <si>
+    <t>2022-Sep-29</t>
+  </si>
+  <si>
+    <t>2022-Sep-30</t>
+  </si>
+  <si>
+    <t>daily1</t>
+  </si>
+  <si>
+    <t>daily2</t>
+  </si>
+  <si>
+    <t>daily3</t>
+  </si>
+  <si>
+    <t>daily4</t>
+  </si>
+  <si>
+    <t>daily5</t>
+  </si>
+  <si>
+    <t>2023Y</t>
+  </si>
+  <si>
+    <t>2024Y</t>
+  </si>
+  <si>
+    <t>2025Y</t>
+  </si>
+  <si>
+    <t>2026Y</t>
+  </si>
+  <si>
+    <t>2027Y</t>
+  </si>
+  <si>
+    <t>2028Y</t>
+  </si>
+  <si>
+    <t>2029Y</t>
+  </si>
+  <si>
+    <t>2030Y</t>
+  </si>
+  <si>
+    <t>2031Y</t>
+  </si>
+  <si>
+    <t>2032Y</t>
+  </si>
+  <si>
+    <t>2033Y</t>
+  </si>
+  <si>
+    <t>2034Y</t>
+  </si>
+  <si>
+    <t>2035Y</t>
+  </si>
+  <si>
+    <t>2036Y</t>
+  </si>
+  <si>
+    <t>2037Y</t>
+  </si>
+  <si>
+    <t>2038Y</t>
+  </si>
+  <si>
+    <t>2039Y</t>
+  </si>
+  <si>
+    <t>2040Y</t>
+  </si>
+  <si>
+    <t>2041Y</t>
+  </si>
+  <si>
+    <t>yearly1</t>
+  </si>
+  <si>
+    <t>yearly2</t>
+  </si>
+  <si>
+    <t>yearly3</t>
+  </si>
+  <si>
+    <t>yearly4</t>
+  </si>
+  <si>
+    <t>yearly5</t>
+  </si>
+  <si>
+    <t>2023H1</t>
+  </si>
+  <si>
+    <t>2023H2</t>
+  </si>
+  <si>
+    <t>2024H1</t>
+  </si>
+  <si>
+    <t>2024H2</t>
+  </si>
+  <si>
+    <t>2025H1</t>
+  </si>
+  <si>
+    <t>2025H2</t>
+  </si>
+  <si>
+    <t>2026H1</t>
+  </si>
+  <si>
+    <t>2026H2</t>
+  </si>
+  <si>
+    <t>2027H1</t>
+  </si>
+  <si>
+    <t>2027H2</t>
+  </si>
+  <si>
+    <t>2028H1</t>
+  </si>
+  <si>
+    <t>2028H2</t>
+  </si>
+  <si>
+    <t>2029H1</t>
+  </si>
+  <si>
+    <t>2029H2</t>
+  </si>
+  <si>
+    <t>2030H1</t>
+  </si>
+  <si>
+    <t>halfyearly1</t>
+  </si>
+  <si>
+    <t>halfyearly2</t>
+  </si>
+  <si>
+    <t>halfyearly3</t>
+  </si>
+  <si>
+    <t>halfyearly4</t>
+  </si>
+  <si>
+    <t>halfyearly5</t>
+  </si>
+  <si>
+    <t>2022Q4</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>quarterly1</t>
+  </si>
+  <si>
+    <t>quarterly2</t>
+  </si>
+  <si>
+    <t>quarterly3</t>
+  </si>
+  <si>
+    <t>quarterly4</t>
+  </si>
+  <si>
+    <t>quarterly5</t>
+  </si>
+  <si>
+    <t>2022M10</t>
+  </si>
+  <si>
+    <t>2022M11</t>
+  </si>
+  <si>
+    <t>2022M12</t>
+  </si>
+  <si>
+    <t>2023M01</t>
+  </si>
+  <si>
+    <t>2023M02</t>
+  </si>
+  <si>
+    <t>2023M03</t>
+  </si>
+  <si>
+    <t>2023M04</t>
+  </si>
+  <si>
+    <t>2023M05</t>
+  </si>
+  <si>
+    <t>2023M06</t>
+  </si>
+  <si>
+    <t>2023M07</t>
+  </si>
+  <si>
+    <t>2023M08</t>
+  </si>
+  <si>
+    <t>2023M09</t>
+  </si>
+  <si>
+    <t>monthly1</t>
+  </si>
+  <si>
+    <t>monthly2</t>
+  </si>
+  <si>
+    <t>monthly3</t>
+  </si>
+  <si>
+    <t>monthly4</t>
+  </si>
+  <si>
+    <t>monthly5</t>
+  </si>
+  <si>
+    <t>2022W39</t>
+  </si>
+  <si>
+    <t>2022W40</t>
+  </si>
+  <si>
+    <t>2022W41</t>
+  </si>
+  <si>
+    <t>2022W42</t>
+  </si>
+  <si>
+    <t>2022W43</t>
+  </si>
+  <si>
+    <t>2022W44</t>
+  </si>
+  <si>
+    <t>2022W45</t>
+  </si>
+  <si>
+    <t>2022W46</t>
+  </si>
+  <si>
+    <t>2022W47</t>
+  </si>
+  <si>
+    <t>2022W48</t>
+  </si>
+  <si>
+    <t>2022W49</t>
+  </si>
+  <si>
+    <t>2022W50</t>
+  </si>
+  <si>
+    <t>2022W51</t>
+  </si>
+  <si>
+    <t>2022W52</t>
+  </si>
+  <si>
+    <t>2023W01</t>
+  </si>
+  <si>
+    <t>2023W02</t>
+  </si>
+  <si>
+    <t>weekly1</t>
+  </si>
+  <si>
+    <t>weekly2</t>
+  </si>
+  <si>
+    <t>weekly3</t>
+  </si>
+  <si>
+    <t>weekly4</t>
+  </si>
+  <si>
+    <t>weekly5</t>
+  </si>
+  <si>
+    <t>2022-Sep-16</t>
+  </si>
+  <si>
+    <t>2022-Sep-17</t>
+  </si>
+  <si>
+    <t>2022-Sep-18</t>
+  </si>
+  <si>
+    <t>2022-Sep-19</t>
+  </si>
+  <si>
+    <t>2022-Sep-20</t>
+  </si>
+  <si>
+    <t>2022-Sep-21</t>
+  </si>
+  <si>
+    <t>2022-Sep-22</t>
+  </si>
+  <si>
+    <t>2022-Sep-23</t>
+  </si>
+  <si>
+    <t>2022-Sep-24</t>
+  </si>
+  <si>
+    <t>2022-Sep-25</t>
+  </si>
+  <si>
+    <t>2022-Sep-26</t>
+  </si>
+  <si>
+    <t>2022-Sep-27</t>
+  </si>
+  <si>
+    <t>2022-Sep-28</t>
+  </si>
+  <si>
+    <t>2022-Sep-29</t>
+  </si>
+  <si>
+    <t>2022-Sep-30</t>
+  </si>
+  <si>
+    <t>daily1</t>
+  </si>
+  <si>
+    <t>daily2</t>
+  </si>
+  <si>
+    <t>daily3</t>
+  </si>
+  <si>
+    <t>daily4</t>
+  </si>
+  <si>
+    <t>daily5</t>
+  </si>
+  <si>
+    <t>2023Y</t>
+  </si>
+  <si>
+    <t>2024Y</t>
+  </si>
+  <si>
+    <t>2025Y</t>
+  </si>
+  <si>
+    <t>2026Y</t>
+  </si>
+  <si>
+    <t>2027Y</t>
+  </si>
+  <si>
+    <t>2028Y</t>
+  </si>
+  <si>
+    <t>2029Y</t>
+  </si>
+  <si>
+    <t>2030Y</t>
+  </si>
+  <si>
+    <t>2031Y</t>
+  </si>
+  <si>
+    <t>2032Y</t>
+  </si>
+  <si>
+    <t>2033Y</t>
+  </si>
+  <si>
+    <t>2034Y</t>
+  </si>
+  <si>
+    <t>2035Y</t>
+  </si>
+  <si>
+    <t>2036Y</t>
+  </si>
+  <si>
+    <t>2037Y</t>
+  </si>
+  <si>
+    <t>2038Y</t>
+  </si>
+  <si>
+    <t>2039Y</t>
+  </si>
+  <si>
+    <t>2040Y</t>
+  </si>
+  <si>
+    <t>2041Y</t>
+  </si>
+  <si>
+    <t>yearly1</t>
+  </si>
+  <si>
+    <t>yearly2</t>
+  </si>
+  <si>
+    <t>yearly3</t>
+  </si>
+  <si>
+    <t>yearly4</t>
+  </si>
+  <si>
+    <t>yearly5</t>
+  </si>
+  <si>
+    <t>2023H1</t>
+  </si>
+  <si>
+    <t>2023H2</t>
+  </si>
+  <si>
+    <t>2024H1</t>
+  </si>
+  <si>
+    <t>2024H2</t>
+  </si>
+  <si>
+    <t>2025H1</t>
+  </si>
+  <si>
+    <t>2025H2</t>
+  </si>
+  <si>
+    <t>2026H1</t>
+  </si>
+  <si>
+    <t>2026H2</t>
+  </si>
+  <si>
+    <t>2027H1</t>
+  </si>
+  <si>
+    <t>2027H2</t>
+  </si>
+  <si>
+    <t>2028H1</t>
+  </si>
+  <si>
+    <t>2028H2</t>
+  </si>
+  <si>
+    <t>2029H1</t>
+  </si>
+  <si>
+    <t>2029H2</t>
+  </si>
+  <si>
+    <t>2030H1</t>
+  </si>
+  <si>
+    <t>halfyearly1</t>
+  </si>
+  <si>
+    <t>halfyearly2</t>
+  </si>
+  <si>
+    <t>halfyearly3</t>
+  </si>
+  <si>
+    <t>halfyearly4</t>
+  </si>
+  <si>
+    <t>halfyearly5</t>
+  </si>
+  <si>
+    <t>2022Q4</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>quarterly1</t>
+  </si>
+  <si>
+    <t>quarterly2</t>
+  </si>
+  <si>
+    <t>quarterly3</t>
+  </si>
+  <si>
+    <t>quarterly4</t>
+  </si>
+  <si>
+    <t>quarterly5</t>
+  </si>
+  <si>
+    <t>2022M10</t>
+  </si>
+  <si>
+    <t>2022M11</t>
+  </si>
+  <si>
+    <t>2022M12</t>
+  </si>
+  <si>
+    <t>2023M01</t>
+  </si>
+  <si>
+    <t>2023M02</t>
+  </si>
+  <si>
+    <t>2023M03</t>
+  </si>
+  <si>
+    <t>2023M04</t>
+  </si>
+  <si>
+    <t>2023M05</t>
+  </si>
+  <si>
+    <t>2023M06</t>
+  </si>
+  <si>
+    <t>2023M07</t>
+  </si>
+  <si>
+    <t>2023M08</t>
+  </si>
+  <si>
+    <t>2023M09</t>
+  </si>
+  <si>
+    <t>monthly1</t>
+  </si>
+  <si>
+    <t>monthly2</t>
+  </si>
+  <si>
+    <t>monthly3</t>
+  </si>
+  <si>
+    <t>monthly4</t>
+  </si>
+  <si>
+    <t>monthly5</t>
+  </si>
+  <si>
+    <t>2022W39</t>
+  </si>
+  <si>
+    <t>2022W40</t>
+  </si>
+  <si>
+    <t>2022W41</t>
+  </si>
+  <si>
+    <t>2022W42</t>
+  </si>
+  <si>
+    <t>2022W43</t>
+  </si>
+  <si>
+    <t>2022W44</t>
+  </si>
+  <si>
+    <t>2022W45</t>
+  </si>
+  <si>
+    <t>2022W46</t>
+  </si>
+  <si>
+    <t>2022W47</t>
+  </si>
+  <si>
+    <t>2022W48</t>
+  </si>
+  <si>
+    <t>2022W49</t>
+  </si>
+  <si>
+    <t>2022W50</t>
+  </si>
+  <si>
+    <t>2022W51</t>
+  </si>
+  <si>
+    <t>2022W52</t>
+  </si>
+  <si>
+    <t>2023W01</t>
+  </si>
+  <si>
+    <t>2023W02</t>
+  </si>
+  <si>
+    <t>weekly1</t>
+  </si>
+  <si>
+    <t>weekly2</t>
+  </si>
+  <si>
+    <t>weekly3</t>
+  </si>
+  <si>
+    <t>weekly4</t>
+  </si>
+  <si>
+    <t>weekly5</t>
+  </si>
+  <si>
+    <t>2022-Sep-19</t>
+  </si>
+  <si>
+    <t>2022-Sep-20</t>
+  </si>
+  <si>
+    <t>2022-Sep-21</t>
+  </si>
+  <si>
+    <t>2022-Sep-22</t>
+  </si>
+  <si>
+    <t>2022-Sep-23</t>
+  </si>
+  <si>
+    <t>2022-Sep-24</t>
+  </si>
+  <si>
+    <t>2022-Sep-25</t>
+  </si>
+  <si>
+    <t>2022-Sep-26</t>
+  </si>
+  <si>
+    <t>2022-Sep-27</t>
+  </si>
+  <si>
+    <t>2022-Sep-28</t>
+  </si>
+  <si>
+    <t>2022-Sep-29</t>
+  </si>
+  <si>
+    <t>2022-Sep-30</t>
+  </si>
+  <si>
+    <t>2022-Oct-01</t>
+  </si>
+  <si>
+    <t>2022-Oct-02</t>
+  </si>
+  <si>
+    <t>2022-Oct-03</t>
+  </si>
+  <si>
+    <t>daily1</t>
+  </si>
+  <si>
+    <t>daily2</t>
+  </si>
+  <si>
+    <t>daily3</t>
+  </si>
+  <si>
+    <t>daily4</t>
+  </si>
+  <si>
+    <t>daily5</t>
+  </si>
+  <si>
+    <t>2023Y</t>
+  </si>
+  <si>
+    <t>2024Y</t>
+  </si>
+  <si>
+    <t>2025Y</t>
+  </si>
+  <si>
+    <t>2026Y</t>
+  </si>
+  <si>
+    <t>2027Y</t>
+  </si>
+  <si>
+    <t>2028Y</t>
+  </si>
+  <si>
+    <t>2029Y</t>
+  </si>
+  <si>
+    <t>2030Y</t>
+  </si>
+  <si>
+    <t>2031Y</t>
+  </si>
+  <si>
+    <t>2032Y</t>
+  </si>
+  <si>
+    <t>2033Y</t>
+  </si>
+  <si>
+    <t>2034Y</t>
+  </si>
+  <si>
+    <t>2035Y</t>
+  </si>
+  <si>
+    <t>2036Y</t>
+  </si>
+  <si>
+    <t>2037Y</t>
+  </si>
+  <si>
+    <t>2038Y</t>
+  </si>
+  <si>
+    <t>2039Y</t>
+  </si>
+  <si>
+    <t>2040Y</t>
+  </si>
+  <si>
+    <t>2041Y</t>
+  </si>
+  <si>
+    <t>yearly1</t>
+  </si>
+  <si>
+    <t>yearly2</t>
+  </si>
+  <si>
+    <t>yearly3</t>
+  </si>
+  <si>
+    <t>yearly4</t>
+  </si>
+  <si>
+    <t>yearly5</t>
+  </si>
+  <si>
+    <t>2023H1</t>
+  </si>
+  <si>
+    <t>2023H2</t>
+  </si>
+  <si>
+    <t>2024H1</t>
+  </si>
+  <si>
+    <t>2024H2</t>
+  </si>
+  <si>
+    <t>2025H1</t>
+  </si>
+  <si>
+    <t>2025H2</t>
+  </si>
+  <si>
+    <t>2026H1</t>
+  </si>
+  <si>
+    <t>2026H2</t>
+  </si>
+  <si>
+    <t>2027H1</t>
+  </si>
+  <si>
+    <t>2027H2</t>
+  </si>
+  <si>
+    <t>2028H1</t>
+  </si>
+  <si>
+    <t>2028H2</t>
+  </si>
+  <si>
+    <t>2029H1</t>
+  </si>
+  <si>
+    <t>2029H2</t>
+  </si>
+  <si>
+    <t>2030H1</t>
+  </si>
+  <si>
+    <t>halfyearly1</t>
+  </si>
+  <si>
+    <t>halfyearly2</t>
+  </si>
+  <si>
+    <t>halfyearly3</t>
+  </si>
+  <si>
+    <t>halfyearly4</t>
+  </si>
+  <si>
+    <t>halfyearly5</t>
+  </si>
+  <si>
+    <t>2022Q4</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>quarterly1</t>
+  </si>
+  <si>
+    <t>quarterly2</t>
+  </si>
+  <si>
+    <t>quarterly3</t>
+  </si>
+  <si>
+    <t>quarterly4</t>
+  </si>
+  <si>
+    <t>quarterly5</t>
+  </si>
+  <si>
+    <t>2022M10</t>
+  </si>
+  <si>
+    <t>2022M11</t>
+  </si>
+  <si>
+    <t>2022M12</t>
+  </si>
+  <si>
+    <t>2023M01</t>
+  </si>
+  <si>
+    <t>2023M02</t>
+  </si>
+  <si>
+    <t>2023M03</t>
+  </si>
+  <si>
+    <t>2023M04</t>
+  </si>
+  <si>
+    <t>2023M05</t>
+  </si>
+  <si>
+    <t>2023M06</t>
+  </si>
+  <si>
+    <t>2023M07</t>
+  </si>
+  <si>
+    <t>2023M08</t>
+  </si>
+  <si>
+    <t>2023M09</t>
+  </si>
+  <si>
+    <t>monthly1</t>
+  </si>
+  <si>
+    <t>monthly2</t>
+  </si>
+  <si>
+    <t>monthly3</t>
+  </si>
+  <si>
+    <t>monthly4</t>
+  </si>
+  <si>
+    <t>monthly5</t>
+  </si>
+  <si>
+    <t>2022W39</t>
+  </si>
+  <si>
+    <t>2022W40</t>
+  </si>
+  <si>
+    <t>2022W41</t>
+  </si>
+  <si>
+    <t>2022W42</t>
+  </si>
+  <si>
+    <t>2022W43</t>
+  </si>
+  <si>
+    <t>2022W44</t>
+  </si>
+  <si>
+    <t>2022W45</t>
+  </si>
+  <si>
+    <t>2022W46</t>
+  </si>
+  <si>
+    <t>2022W47</t>
+  </si>
+  <si>
+    <t>2022W48</t>
+  </si>
+  <si>
+    <t>2022W49</t>
+  </si>
+  <si>
+    <t>2022W50</t>
+  </si>
+  <si>
+    <t>2022W51</t>
+  </si>
+  <si>
+    <t>2022W52</t>
+  </si>
+  <si>
+    <t>2023W01</t>
+  </si>
+  <si>
+    <t>2023W02</t>
+  </si>
+  <si>
+    <t>weekly1</t>
+  </si>
+  <si>
+    <t>weekly2</t>
+  </si>
+  <si>
+    <t>weekly3</t>
+  </si>
+  <si>
+    <t>weekly4</t>
+  </si>
+  <si>
+    <t>weekly5</t>
+  </si>
+  <si>
+    <t>2022-Sep-19</t>
+  </si>
+  <si>
+    <t>2022-Sep-20</t>
+  </si>
+  <si>
+    <t>2022-Sep-21</t>
+  </si>
+  <si>
+    <t>2022-Sep-22</t>
+  </si>
+  <si>
+    <t>2022-Sep-23</t>
+  </si>
+  <si>
+    <t>2022-Sep-24</t>
+  </si>
+  <si>
+    <t>2022-Sep-25</t>
+  </si>
+  <si>
+    <t>2022-Sep-26</t>
+  </si>
+  <si>
+    <t>2022-Sep-27</t>
+  </si>
+  <si>
+    <t>2022-Sep-28</t>
+  </si>
+  <si>
+    <t>2022-Sep-29</t>
+  </si>
+  <si>
+    <t>2022-Sep-30</t>
+  </si>
+  <si>
+    <t>2022-Oct-01</t>
+  </si>
+  <si>
+    <t>2022-Oct-02</t>
+  </si>
+  <si>
+    <t>2022-Oct-03</t>
+  </si>
+  <si>
+    <t>daily1</t>
+  </si>
+  <si>
+    <t>daily2</t>
+  </si>
+  <si>
+    <t>daily3</t>
+  </si>
+  <si>
+    <t>daily4</t>
+  </si>
+  <si>
+    <t>daily5</t>
+  </si>
+  <si>
+    <t>2023Y</t>
+  </si>
+  <si>
+    <t>2024Y</t>
+  </si>
+  <si>
+    <t>2025Y</t>
+  </si>
+  <si>
+    <t>2026Y</t>
+  </si>
+  <si>
+    <t>2027Y</t>
+  </si>
+  <si>
+    <t>2028Y</t>
+  </si>
+  <si>
+    <t>2029Y</t>
+  </si>
+  <si>
+    <t>2030Y</t>
+  </si>
+  <si>
+    <t>2031Y</t>
+  </si>
+  <si>
+    <t>2032Y</t>
+  </si>
+  <si>
+    <t>2033Y</t>
+  </si>
+  <si>
+    <t>2034Y</t>
+  </si>
+  <si>
+    <t>2035Y</t>
+  </si>
+  <si>
+    <t>2036Y</t>
+  </si>
+  <si>
+    <t>2037Y</t>
+  </si>
+  <si>
+    <t>2038Y</t>
+  </si>
+  <si>
+    <t>2039Y</t>
+  </si>
+  <si>
+    <t>2040Y</t>
+  </si>
+  <si>
+    <t>2041Y</t>
+  </si>
+  <si>
+    <t>yearly1</t>
+  </si>
+  <si>
+    <t>yearly2</t>
+  </si>
+  <si>
+    <t>yearly3</t>
+  </si>
+  <si>
+    <t>yearly4</t>
+  </si>
+  <si>
+    <t>yearly5</t>
+  </si>
+  <si>
+    <t>2023H1</t>
+  </si>
+  <si>
+    <t>2023H2</t>
+  </si>
+  <si>
+    <t>2024H1</t>
+  </si>
+  <si>
+    <t>2024H2</t>
+  </si>
+  <si>
+    <t>2025H1</t>
+  </si>
+  <si>
+    <t>2025H2</t>
+  </si>
+  <si>
+    <t>2026H1</t>
+  </si>
+  <si>
+    <t>2026H2</t>
+  </si>
+  <si>
+    <t>2027H1</t>
+  </si>
+  <si>
+    <t>2027H2</t>
+  </si>
+  <si>
+    <t>2028H1</t>
+  </si>
+  <si>
+    <t>2028H2</t>
+  </si>
+  <si>
+    <t>2029H1</t>
+  </si>
+  <si>
+    <t>2029H2</t>
+  </si>
+  <si>
+    <t>2030H1</t>
+  </si>
+  <si>
+    <t>halfyearly1</t>
+  </si>
+  <si>
+    <t>halfyearly2</t>
+  </si>
+  <si>
+    <t>halfyearly3</t>
+  </si>
+  <si>
+    <t>halfyearly4</t>
+  </si>
+  <si>
+    <t>halfyearly5</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>2025Q2</t>
+  </si>
+  <si>
+    <t>quarterly1</t>
+  </si>
+  <si>
+    <t>quarterly2</t>
+  </si>
+  <si>
+    <t>quarterly3</t>
+  </si>
+  <si>
+    <t>quarterly4</t>
+  </si>
+  <si>
+    <t>quarterly5</t>
+  </si>
+  <si>
+    <t>2022M11</t>
+  </si>
+  <si>
+    <t>2022M12</t>
+  </si>
+  <si>
+    <t>2023M01</t>
+  </si>
+  <si>
+    <t>2023M02</t>
+  </si>
+  <si>
+    <t>2023M03</t>
+  </si>
+  <si>
+    <t>2023M04</t>
+  </si>
+  <si>
+    <t>2023M05</t>
+  </si>
+  <si>
+    <t>2023M06</t>
+  </si>
+  <si>
+    <t>2023M07</t>
+  </si>
+  <si>
+    <t>2023M08</t>
+  </si>
+  <si>
+    <t>2023M09</t>
+  </si>
+  <si>
+    <t>2023M10</t>
+  </si>
+  <si>
+    <t>monthly1</t>
+  </si>
+  <si>
+    <t>monthly2</t>
+  </si>
+  <si>
+    <t>monthly3</t>
+  </si>
+  <si>
+    <t>monthly4</t>
+  </si>
+  <si>
+    <t>monthly5</t>
+  </si>
+  <si>
+    <t>2022W43</t>
+  </si>
+  <si>
+    <t>2022W44</t>
+  </si>
+  <si>
+    <t>2022W45</t>
+  </si>
+  <si>
+    <t>2022W46</t>
+  </si>
+  <si>
+    <t>2022W47</t>
+  </si>
+  <si>
+    <t>2022W48</t>
+  </si>
+  <si>
+    <t>2022W49</t>
+  </si>
+  <si>
+    <t>2022W50</t>
+  </si>
+  <si>
+    <t>2022W51</t>
+  </si>
+  <si>
+    <t>2022W52</t>
+  </si>
+  <si>
+    <t>2023W01</t>
+  </si>
+  <si>
+    <t>2023W02</t>
+  </si>
+  <si>
+    <t>2023W03</t>
+  </si>
+  <si>
+    <t>2023W04</t>
+  </si>
+  <si>
+    <t>2023W05</t>
+  </si>
+  <si>
+    <t>2023W06</t>
+  </si>
+  <si>
+    <t>weekly1</t>
+  </si>
+  <si>
+    <t>weekly2</t>
+  </si>
+  <si>
+    <t>weekly3</t>
+  </si>
+  <si>
+    <t>weekly4</t>
+  </si>
+  <si>
+    <t>weekly5</t>
+  </si>
+  <si>
+    <t>2022-Oct-17</t>
+  </si>
+  <si>
+    <t>2022-Oct-18</t>
+  </si>
+  <si>
+    <t>2022-Oct-19</t>
+  </si>
+  <si>
+    <t>2022-Oct-20</t>
+  </si>
+  <si>
+    <t>2022-Oct-21</t>
+  </si>
+  <si>
+    <t>2022-Oct-22</t>
+  </si>
+  <si>
+    <t>2022-Oct-23</t>
+  </si>
+  <si>
+    <t>2022-Oct-24</t>
+  </si>
+  <si>
+    <t>2022-Oct-25</t>
+  </si>
+  <si>
+    <t>2022-Oct-26</t>
+  </si>
+  <si>
+    <t>2022-Oct-27</t>
+  </si>
+  <si>
+    <t>2022-Oct-28</t>
+  </si>
+  <si>
+    <t>2022-Oct-29</t>
+  </si>
+  <si>
+    <t>2022-Oct-30</t>
+  </si>
+  <si>
+    <t>2022-Oct-31</t>
+  </si>
+  <si>
+    <t>daily1</t>
+  </si>
+  <si>
+    <t>daily2</t>
+  </si>
+  <si>
+    <t>daily3</t>
+  </si>
+  <si>
+    <t>daily4</t>
+  </si>
+  <si>
+    <t>daily5</t>
+  </si>
+  <si>
+    <t>2023Y</t>
+  </si>
+  <si>
+    <t>2024Y</t>
+  </si>
+  <si>
+    <t>2025Y</t>
+  </si>
+  <si>
+    <t>2026Y</t>
+  </si>
+  <si>
+    <t>2027Y</t>
+  </si>
+  <si>
+    <t>2028Y</t>
+  </si>
+  <si>
+    <t>2029Y</t>
+  </si>
+  <si>
+    <t>2030Y</t>
+  </si>
+  <si>
+    <t>2031Y</t>
+  </si>
+  <si>
+    <t>2032Y</t>
+  </si>
+  <si>
+    <t>2033Y</t>
+  </si>
+  <si>
+    <t>2034Y</t>
+  </si>
+  <si>
+    <t>2035Y</t>
+  </si>
+  <si>
+    <t>2036Y</t>
+  </si>
+  <si>
+    <t>2037Y</t>
+  </si>
+  <si>
+    <t>2038Y</t>
+  </si>
+  <si>
+    <t>2039Y</t>
+  </si>
+  <si>
+    <t>2040Y</t>
+  </si>
+  <si>
+    <t>2041Y</t>
+  </si>
+  <si>
+    <t>yearly1</t>
+  </si>
+  <si>
+    <t>yearly2</t>
+  </si>
+  <si>
+    <t>yearly3</t>
+  </si>
+  <si>
+    <t>yearly4</t>
+  </si>
+  <si>
+    <t>yearly5</t>
+  </si>
+  <si>
+    <t>2023H1</t>
+  </si>
+  <si>
+    <t>2023H2</t>
+  </si>
+  <si>
+    <t>2024H1</t>
+  </si>
+  <si>
+    <t>2024H2</t>
+  </si>
+  <si>
+    <t>2025H1</t>
+  </si>
+  <si>
+    <t>2025H2</t>
+  </si>
+  <si>
+    <t>2026H1</t>
+  </si>
+  <si>
+    <t>2026H2</t>
+  </si>
+  <si>
+    <t>2027H1</t>
+  </si>
+  <si>
+    <t>2027H2</t>
+  </si>
+  <si>
+    <t>2028H1</t>
+  </si>
+  <si>
+    <t>2028H2</t>
+  </si>
+  <si>
+    <t>2029H1</t>
+  </si>
+  <si>
+    <t>2029H2</t>
+  </si>
+  <si>
+    <t>2030H1</t>
+  </si>
+  <si>
+    <t>halfyearly1</t>
+  </si>
+  <si>
+    <t>halfyearly2</t>
+  </si>
+  <si>
+    <t>halfyearly3</t>
+  </si>
+  <si>
+    <t>halfyearly4</t>
+  </si>
+  <si>
+    <t>halfyearly5</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>2025Q2</t>
+  </si>
+  <si>
+    <t>quarterly1</t>
+  </si>
+  <si>
+    <t>quarterly2</t>
+  </si>
+  <si>
+    <t>quarterly3</t>
+  </si>
+  <si>
+    <t>quarterly4</t>
+  </si>
+  <si>
+    <t>quarterly5</t>
+  </si>
+  <si>
+    <t>2022M11</t>
+  </si>
+  <si>
+    <t>2022M12</t>
+  </si>
+  <si>
+    <t>2023M01</t>
+  </si>
+  <si>
+    <t>2023M02</t>
+  </si>
+  <si>
+    <t>2023M03</t>
+  </si>
+  <si>
+    <t>2023M04</t>
+  </si>
+  <si>
+    <t>2023M05</t>
+  </si>
+  <si>
+    <t>2023M06</t>
+  </si>
+  <si>
+    <t>2023M07</t>
+  </si>
+  <si>
+    <t>2023M08</t>
+  </si>
+  <si>
+    <t>2023M09</t>
+  </si>
+  <si>
+    <t>2023M10</t>
+  </si>
+  <si>
+    <t>monthly1</t>
+  </si>
+  <si>
+    <t>monthly2</t>
+  </si>
+  <si>
+    <t>monthly3</t>
+  </si>
+  <si>
+    <t>monthly4</t>
+  </si>
+  <si>
+    <t>monthly5</t>
+  </si>
+  <si>
+    <t>2022W43</t>
+  </si>
+  <si>
+    <t>2022W44</t>
+  </si>
+  <si>
+    <t>2022W45</t>
+  </si>
+  <si>
+    <t>2022W46</t>
+  </si>
+  <si>
+    <t>2022W47</t>
+  </si>
+  <si>
+    <t>2022W48</t>
+  </si>
+  <si>
+    <t>2022W49</t>
+  </si>
+  <si>
+    <t>2022W50</t>
+  </si>
+  <si>
+    <t>2022W51</t>
+  </si>
+  <si>
+    <t>2022W52</t>
+  </si>
+  <si>
+    <t>2023W01</t>
+  </si>
+  <si>
+    <t>2023W02</t>
+  </si>
+  <si>
+    <t>2023W03</t>
+  </si>
+  <si>
+    <t>2023W04</t>
+  </si>
+  <si>
+    <t>2023W05</t>
+  </si>
+  <si>
+    <t>2023W06</t>
+  </si>
+  <si>
+    <t>weekly1</t>
+  </si>
+  <si>
+    <t>weekly2</t>
+  </si>
+  <si>
+    <t>weekly3</t>
+  </si>
+  <si>
+    <t>weekly4</t>
+  </si>
+  <si>
+    <t>weekly5</t>
+  </si>
+  <si>
+    <t>2022-Oct-17</t>
+  </si>
+  <si>
+    <t>2022-Oct-18</t>
+  </si>
+  <si>
+    <t>2022-Oct-19</t>
+  </si>
+  <si>
+    <t>2022-Oct-20</t>
+  </si>
+  <si>
+    <t>2022-Oct-21</t>
+  </si>
+  <si>
+    <t>2022-Oct-22</t>
+  </si>
+  <si>
+    <t>2022-Oct-23</t>
+  </si>
+  <si>
+    <t>2022-Oct-24</t>
+  </si>
+  <si>
+    <t>2022-Oct-25</t>
+  </si>
+  <si>
+    <t>2022-Oct-26</t>
+  </si>
+  <si>
+    <t>2022-Oct-27</t>
+  </si>
+  <si>
+    <t>2022-Oct-28</t>
+  </si>
+  <si>
+    <t>2022-Oct-29</t>
+  </si>
+  <si>
+    <t>2022-Oct-30</t>
+  </si>
+  <si>
+    <t>2022-Oct-31</t>
   </si>
   <si>
     <t>daily1</t>
@@ -16138,7 +18595,7 @@
   <dimension ref="A1:F16"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="true"/>
+    <col min="1" max="1" width="11.5703125" customWidth="true"/>
     <col min="2" max="2" width="14.7109375" customWidth="true"/>
     <col min="3" max="3" width="13.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
@@ -16149,24 +18606,24 @@
     <row r="1">
       <c r="A1" s="0"/>
       <c r="B1" s="0" t="s">
-        <v>5352</v>
+        <v>6171</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5353</v>
+        <v>6172</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5354</v>
+        <v>6173</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5355</v>
+        <v>6174</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5356</v>
+        <v>6175</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5337</v>
+        <v>6156</v>
       </c>
       <c r="B2" s="0">
         <v>0.0077822300572673031</v>
@@ -16180,7 +18637,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5338</v>
+        <v>6157</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="0"/>
@@ -16194,7 +18651,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>5339</v>
+        <v>6158</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
@@ -16208,7 +18665,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>5340</v>
+        <v>6159</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0">
@@ -16226,7 +18683,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5341</v>
+        <v>6160</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0">
@@ -16244,7 +18701,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>5342</v>
+        <v>6161</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0">
@@ -16260,7 +18717,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>5343</v>
+        <v>6162</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0">
@@ -16276,7 +18733,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>5344</v>
+        <v>6163</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0">
@@ -16292,7 +18749,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>5345</v>
+        <v>6164</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0">
@@ -16306,7 +18763,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>5346</v>
+        <v>6165</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0">
@@ -16320,7 +18777,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>5347</v>
+        <v>6166</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0">
@@ -16334,7 +18791,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>5348</v>
+        <v>6167</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0">
@@ -16348,7 +18805,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>5349</v>
+        <v>6168</v>
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="0">
@@ -16362,7 +18819,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>5350</v>
+        <v>6169</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0">
@@ -16376,7 +18833,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>5351</v>
+        <v>6170</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -16406,24 +18863,24 @@
     <row r="1">
       <c r="A1" s="0"/>
       <c r="B1" s="0" t="s">
-        <v>5259</v>
+        <v>6078</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5260</v>
+        <v>6079</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5261</v>
+        <v>6080</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5262</v>
+        <v>6081</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5263</v>
+        <v>6082</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5240</v>
+        <v>6059</v>
       </c>
       <c r="B2" s="0">
         <v>0.44573095817754427</v>
@@ -16435,7 +18892,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5241</v>
+        <v>6060</v>
       </c>
       <c r="B3" s="0">
         <v>0.93884503662500751</v>
@@ -16451,7 +18908,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>5242</v>
+        <v>6061</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
@@ -16465,7 +18922,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>5243</v>
+        <v>6062</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="0">
@@ -16481,7 +18938,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5244</v>
+        <v>6063</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0">
@@ -16497,7 +18954,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>5245</v>
+        <v>6064</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0">
@@ -16511,7 +18968,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>5246</v>
+        <v>6065</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0">
@@ -16525,7 +18982,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>5247</v>
+        <v>6066</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0">
@@ -16539,7 +18996,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>5248</v>
+        <v>6067</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0">
@@ -16553,7 +19010,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>5249</v>
+        <v>6068</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0">
@@ -16567,7 +19024,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>5250</v>
+        <v>6069</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0">
@@ -16581,7 +19038,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>5251</v>
+        <v>6070</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0">
@@ -16595,7 +19052,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>5252</v>
+        <v>6071</v>
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="0">
@@ -16609,7 +19066,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>5253</v>
+        <v>6072</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0">
@@ -16623,7 +19080,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>5254</v>
+        <v>6073</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0">
@@ -16637,7 +19094,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>5255</v>
+        <v>6074</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0">
@@ -16651,7 +19108,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>5256</v>
+        <v>6075</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0">
@@ -16665,7 +19122,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>5257</v>
+        <v>6076</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
@@ -16677,7 +19134,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>5258</v>
+        <v>6077</v>
       </c>
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
@@ -16707,24 +19164,24 @@
     <row r="1">
       <c r="A1" s="0"/>
       <c r="B1" s="0" t="s">
-        <v>5279</v>
+        <v>6098</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5280</v>
+        <v>6099</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5281</v>
+        <v>6100</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5282</v>
+        <v>6101</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5283</v>
+        <v>6102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5264</v>
+        <v>6083</v>
       </c>
       <c r="B2" s="0">
         <v>0.95912755887763146</v>
@@ -16736,7 +19193,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5265</v>
+        <v>6084</v>
       </c>
       <c r="B3" s="0">
         <v>0.15599623700921006</v>
@@ -16750,7 +19207,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>5266</v>
+        <v>6085</v>
       </c>
       <c r="B4" s="0">
         <v>0.92893566527503146</v>
@@ -16768,7 +19225,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>5267</v>
+        <v>6086</v>
       </c>
       <c r="B5" s="0">
         <v>0.42457418676747516</v>
@@ -16786,7 +19243,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5268</v>
+        <v>6087</v>
       </c>
       <c r="B6" s="0">
         <v>0.22308394507279783</v>
@@ -16804,7 +19261,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>5269</v>
+        <v>6088</v>
       </c>
       <c r="B7" s="0">
         <v>0.13639509258625593</v>
@@ -16822,7 +19279,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>5270</v>
+        <v>6089</v>
       </c>
       <c r="B8" s="0">
         <v>0.26017565411199783</v>
@@ -16840,7 +19297,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>5271</v>
+        <v>6090</v>
       </c>
       <c r="B9" s="0">
         <v>0.54446538298976221</v>
@@ -16858,7 +19315,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>5272</v>
+        <v>6091</v>
       </c>
       <c r="B10" s="0">
         <v>0.08220839201942487</v>
@@ -16876,7 +19333,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>5273</v>
+        <v>6092</v>
       </c>
       <c r="B11" s="0">
         <v>0.59812731332654612</v>
@@ -16894,7 +19351,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>5274</v>
+        <v>6093</v>
       </c>
       <c r="B12" s="0">
         <v>0.029186178399368323</v>
@@ -16908,7 +19365,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>5275</v>
+        <v>6094</v>
       </c>
       <c r="B13" s="0">
         <v>0.45490889768790432</v>
@@ -16922,7 +19379,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>5276</v>
+        <v>6095</v>
       </c>
       <c r="B14" s="0">
         <v>0.33249868418860995</v>
@@ -16934,7 +19391,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>5277</v>
+        <v>6096</v>
       </c>
       <c r="B15" s="0">
         <v>0.9436728315558397</v>
@@ -16946,7 +19403,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>5278</v>
+        <v>6097</v>
       </c>
       <c r="B16" s="0">
         <v>0.30310182000969277</v>
@@ -16976,24 +19433,24 @@
     <row r="1">
       <c r="A1" s="0"/>
       <c r="B1" s="0" t="s">
-        <v>5294</v>
+        <v>6113</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5295</v>
+        <v>6114</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5296</v>
+        <v>6115</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5297</v>
+        <v>6116</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5298</v>
+        <v>6117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5284</v>
+        <v>6103</v>
       </c>
       <c r="B2" s="0">
         <v>0.36131340195220318</v>
@@ -17005,7 +19462,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5285</v>
+        <v>6104</v>
       </c>
       <c r="B3" s="0">
         <v>0.47000049054799409</v>
@@ -17021,7 +19478,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>5286</v>
+        <v>6105</v>
       </c>
       <c r="B4" s="0">
         <v>0.058779768820967915</v>
@@ -17039,7 +19496,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>5287</v>
+        <v>6106</v>
       </c>
       <c r="B5" s="0">
         <v>0.33001170117311762</v>
@@ -17057,7 +19514,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5288</v>
+        <v>6107</v>
       </c>
       <c r="B6" s="0">
         <v>0.2645204776577964</v>
@@ -17077,7 +19534,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>5289</v>
+        <v>6108</v>
       </c>
       <c r="B7" s="0">
         <v>0.24591766636495149</v>
@@ -17095,7 +19552,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>5290</v>
+        <v>6109</v>
       </c>
       <c r="B8" s="0">
         <v>0.94767635939633654</v>
@@ -17113,7 +19570,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>5291</v>
+        <v>6110</v>
       </c>
       <c r="B9" s="0">
         <v>0.032441994505736038</v>
@@ -17131,7 +19588,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>5292</v>
+        <v>6111</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0">
@@ -17145,7 +19602,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>5293</v>
+        <v>6112</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0">
@@ -17175,24 +19632,24 @@
     <row r="1">
       <c r="A1" s="0"/>
       <c r="B1" s="0" t="s">
-        <v>5311</v>
+        <v>6130</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5312</v>
+        <v>6131</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5313</v>
+        <v>6132</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5314</v>
+        <v>6133</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5315</v>
+        <v>6134</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5299</v>
+        <v>6118</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
@@ -17204,7 +19661,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5300</v>
+        <v>6119</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="0"/>
@@ -17218,7 +19675,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>5301</v>
+        <v>6120</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
@@ -17232,7 +19689,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>5302</v>
+        <v>6121</v>
       </c>
       <c r="B5" s="0">
         <v>0.25842844529664455</v>
@@ -17248,7 +19705,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5303</v>
+        <v>6122</v>
       </c>
       <c r="B6" s="0">
         <v>0.41674615988017316</v>
@@ -17264,7 +19721,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>5304</v>
+        <v>6123</v>
       </c>
       <c r="B7" s="0">
         <v>0.38205553895575395</v>
@@ -17280,7 +19737,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>5305</v>
+        <v>6124</v>
       </c>
       <c r="B8" s="0">
         <v>0.096334132994130295</v>
@@ -17294,7 +19751,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>5306</v>
+        <v>6125</v>
       </c>
       <c r="B9" s="0">
         <v>0.13128421939369728</v>
@@ -17308,7 +19765,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>5307</v>
+        <v>6126</v>
       </c>
       <c r="B10" s="0">
         <v>0.60989827041754752</v>
@@ -17322,7 +19779,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>5308</v>
+        <v>6127</v>
       </c>
       <c r="B11" s="0">
         <v>0.65619373187934471</v>
@@ -17336,7 +19793,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>5309</v>
+        <v>6128</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0">
@@ -17348,7 +19805,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>5310</v>
+        <v>6129</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0">
@@ -17378,24 +19835,24 @@
     <row r="1">
       <c r="A1" s="0"/>
       <c r="B1" s="0" t="s">
-        <v>5332</v>
+        <v>6151</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5333</v>
+        <v>6152</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>5334</v>
+        <v>6153</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5335</v>
+        <v>6154</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5336</v>
+        <v>6155</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5316</v>
+        <v>6135</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
@@ -17407,7 +19864,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>5317</v>
+        <v>6136</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="0"/>
@@ -17419,7 +19876,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>5318</v>
+        <v>6137</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0">
@@ -17435,7 +19892,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>5319</v>
+        <v>6138</v>
       </c>
       <c r="B5" s="0">
         <v>0.097101989426797264</v>
@@ -17453,7 +19910,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5320</v>
+        <v>6139</v>
       </c>
       <c r="B6" s="0">
         <v>0.78282152667052363</v>
@@ -17471,7 +19928,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>5321</v>
+        <v>6140</v>
       </c>
       <c r="B7" s="0">
         <v>0.66752094460457012</v>
@@ -17489,7 +19946,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>5322</v>
+        <v>6141</v>
       </c>
       <c r="B8" s="0">
         <v>0.61267254852844133</v>
@@ -17505,7 +19962,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>5323</v>
+        <v>6142</v>
       </c>
       <c r="B9" s="0">
         <v>0.34379242128970755</v>
@@ -17521,7 +19978,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>5324</v>
+        <v>6143</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0"/>
@@ -17535,7 +19992,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>5325</v>
+        <v>6144</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -17549,7 +20006,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>5326</v>
+        <v>6145</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
@@ -17563,7 +20020,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>5327</v>
+        <v>6146</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
@@ -17577,7 +20034,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>5328</v>
+        <v>6147</v>
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="0"/>
@@ -17591,7 +20048,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>5329</v>
+        <v>6148</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0"/>
@@ -17605,7 +20062,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>5330</v>
+        <v>6149</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
@@ -17617,7 +20074,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>5331</v>
+        <v>6150</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0"/>

</xml_diff>